<commit_message>
completed dZAP1 input sheet
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/15-genes_27-edges_BK-dZAP1-fam_no-strains-added_Sigmoid_estimation.xlsx
+++ b/data/GRNmap_input_workbooks/15-genes_27-edges_BK-dZAP1-fam_no-strains-added_Sigmoid_estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="0" windowWidth="25120" windowHeight="15040" tabRatio="500" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="40">
   <si>
     <t>CIN5</t>
   </si>
@@ -141,6 +141,12 @@
   <si>
     <t>dzap1</t>
   </si>
+  <si>
+    <t>optimization_parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
 </sst>
 </file>
 
@@ -208,7 +214,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="237">
+  <cellStyleXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -446,19 +452,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="237">
+  <cellStyles count="239">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -577,6 +587,7 @@
     <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -695,30 +706,10 @@
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -1067,7 +1058,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1">
@@ -1075,7 +1066,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1">
@@ -1083,7 +1074,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1">
@@ -1091,7 +1082,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="1">
@@ -1099,7 +1090,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1">
@@ -1107,7 +1098,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1">
@@ -1115,7 +1106,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1">
@@ -1123,7 +1114,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1">
@@ -1131,7 +1122,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="1">
@@ -1139,7 +1130,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1">
@@ -1147,7 +1138,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1">
@@ -1155,7 +1146,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="1">
@@ -1163,7 +1154,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="1">
@@ -1171,7 +1162,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="1">
@@ -1179,7 +1170,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="1">
@@ -1221,7 +1212,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1">
@@ -1229,7 +1220,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1">
@@ -1237,7 +1228,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1">
@@ -1245,7 +1236,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="1">
@@ -1253,7 +1244,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1">
@@ -1261,7 +1252,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1">
@@ -1269,7 +1260,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1">
@@ -1277,7 +1268,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1">
@@ -1285,7 +1276,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="1">
@@ -1293,7 +1284,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1">
@@ -1301,7 +1292,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1">
@@ -1309,7 +1300,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="1">
@@ -1317,7 +1308,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="1">
@@ -1325,7 +1316,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="1">
@@ -1333,7 +1324,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="1">
@@ -1409,7 +1400,7 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1">
@@ -1453,7 +1444,7 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="2">
@@ -1471,7 +1462,7 @@
       <c r="F3" s="2">
         <v>0.5827</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>-2.52E-2</v>
       </c>
       <c r="H3" s="2">
@@ -1497,7 +1488,7 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2">
@@ -1541,7 +1532,7 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="1">
@@ -1585,7 +1576,7 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2">
@@ -1629,7 +1620,7 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2">
@@ -1673,7 +1664,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2">
@@ -1717,7 +1708,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2">
@@ -1761,7 +1752,7 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="1">
@@ -1805,7 +1796,7 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="2">
@@ -1849,7 +1840,7 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1">
@@ -1893,7 +1884,7 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="1">
@@ -1937,7 +1928,7 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2">
@@ -1981,7 +1972,7 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="2">
@@ -2025,7 +2016,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="2">
@@ -2064,7 +2055,7 @@
       <c r="M16" s="2">
         <v>1.3863000000000001</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="6">
         <v>2.6345999999999998</v>
       </c>
     </row>
@@ -2134,7 +2125,7 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1">
@@ -2175,7 +2166,7 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1">
@@ -2216,10 +2207,10 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
         <v>1.4439</v>
       </c>
       <c r="C4" s="1">
@@ -2257,7 +2248,7 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="1">
@@ -2269,10 +2260,10 @@
       <c r="D5" s="1">
         <v>0.64429999999999998</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>0.96760000000000002</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>0.72609999999999997</v>
       </c>
       <c r="G5" s="1">
@@ -2298,7 +2289,7 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1">
@@ -2339,7 +2330,7 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1">
@@ -2380,7 +2371,7 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1">
@@ -2421,7 +2412,7 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1">
@@ -2462,7 +2453,7 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="1">
@@ -2503,7 +2494,7 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1">
@@ -2544,7 +2535,7 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1">
@@ -2585,7 +2576,7 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="1">
@@ -2626,7 +2617,7 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="1">
@@ -2656,7 +2647,7 @@
       <c r="J14" s="1">
         <v>-0.68630000000000002</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="7">
         <v>1E-4</v>
       </c>
       <c r="L14" s="1">
@@ -2667,7 +2658,7 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="1">
@@ -2708,10 +2699,10 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>0.54390000000000005</v>
       </c>
       <c r="C16" s="1">
@@ -2735,7 +2726,7 @@
       <c r="I16" s="1">
         <v>-0.23730000000000001</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="3">
         <v>-0.93640000000000001</v>
       </c>
       <c r="K16" s="1">
@@ -2776,799 +2767,799 @@
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0</v>
-      </c>
-      <c r="K2" s="6">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6">
-        <v>0</v>
-      </c>
-      <c r="M2" s="6">
-        <v>0</v>
-      </c>
-      <c r="N2" s="6">
-        <v>0</v>
-      </c>
-      <c r="O2" s="6">
-        <v>0</v>
-      </c>
-      <c r="P2" s="6">
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0</v>
+      </c>
+      <c r="P2" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0</v>
-      </c>
-      <c r="M3" s="6">
-        <v>0</v>
-      </c>
-      <c r="N3" s="6">
-        <v>0</v>
-      </c>
-      <c r="O3" s="6">
-        <v>0</v>
-      </c>
-      <c r="P3" s="6">
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>1</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>1</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
-      <c r="O4" s="6">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6">
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0</v>
-      </c>
-      <c r="O6" s="6">
-        <v>0</v>
-      </c>
-      <c r="P6" s="6">
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0</v>
-      </c>
-      <c r="K7" s="6">
-        <v>0</v>
-      </c>
-      <c r="L7" s="6">
-        <v>0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0</v>
-      </c>
-      <c r="N7" s="6">
-        <v>0</v>
-      </c>
-      <c r="O7" s="6">
-        <v>0</v>
-      </c>
-      <c r="P7" s="6">
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1</v>
-      </c>
-      <c r="L8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="6">
-        <v>1</v>
-      </c>
-      <c r="N8" s="6">
-        <v>0</v>
-      </c>
-      <c r="O8" s="6">
-        <v>1</v>
-      </c>
-      <c r="P8" s="6">
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1</v>
+      </c>
+      <c r="P8" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <v>1</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
-        <v>0</v>
-      </c>
-      <c r="L9" s="6">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0</v>
-      </c>
-      <c r="O9" s="6">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6">
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="5">
+        <v>0</v>
+      </c>
+      <c r="P9" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6">
-        <v>0</v>
-      </c>
-      <c r="N10" s="6">
-        <v>0</v>
-      </c>
-      <c r="O10" s="6">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6">
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6">
-        <v>1</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
-        <v>0</v>
-      </c>
-      <c r="N11" s="6">
-        <v>0</v>
-      </c>
-      <c r="O11" s="6">
-        <v>0</v>
-      </c>
-      <c r="P11" s="6">
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="5">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="6">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6">
-        <v>1</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0</v>
-      </c>
-      <c r="K12" s="6">
-        <v>1</v>
-      </c>
-      <c r="L12" s="6">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
-        <v>1</v>
-      </c>
-      <c r="N12" s="6">
-        <v>0</v>
-      </c>
-      <c r="O12" s="6">
-        <v>0</v>
-      </c>
-      <c r="P12" s="6">
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>1</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="O12" s="5">
+        <v>0</v>
+      </c>
+      <c r="P12" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="6">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
-        <v>0</v>
-      </c>
-      <c r="I13" s="6">
-        <v>0</v>
-      </c>
-      <c r="J13" s="6">
-        <v>0</v>
-      </c>
-      <c r="K13" s="6">
-        <v>1</v>
-      </c>
-      <c r="L13" s="6">
-        <v>0</v>
-      </c>
-      <c r="M13" s="6">
-        <v>0</v>
-      </c>
-      <c r="N13" s="6">
-        <v>0</v>
-      </c>
-      <c r="O13" s="6">
-        <v>1</v>
-      </c>
-      <c r="P13" s="6">
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5">
+        <v>1</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+      <c r="O13" s="5">
+        <v>1</v>
+      </c>
+      <c r="P13" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6">
-        <v>1</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0</v>
-      </c>
-      <c r="I14" s="6">
-        <v>0</v>
-      </c>
-      <c r="J14" s="6">
-        <v>0</v>
-      </c>
-      <c r="K14" s="6">
-        <v>1</v>
-      </c>
-      <c r="L14" s="6">
-        <v>0</v>
-      </c>
-      <c r="M14" s="6">
-        <v>0</v>
-      </c>
-      <c r="N14" s="6">
-        <v>0</v>
-      </c>
-      <c r="O14" s="6">
-        <v>0</v>
-      </c>
-      <c r="P14" s="6">
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5">
+        <v>1</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+      <c r="O14" s="5">
+        <v>0</v>
+      </c>
+      <c r="P14" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="6">
-        <v>1</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0</v>
-      </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0</v>
-      </c>
-      <c r="I15" s="6">
-        <v>0</v>
-      </c>
-      <c r="J15" s="6">
-        <v>0</v>
-      </c>
-      <c r="K15" s="6">
-        <v>1</v>
-      </c>
-      <c r="L15" s="6">
-        <v>0</v>
-      </c>
-      <c r="M15" s="6">
-        <v>0</v>
-      </c>
-      <c r="N15" s="6">
-        <v>0</v>
-      </c>
-      <c r="O15" s="6">
-        <v>0</v>
-      </c>
-      <c r="P15" s="6">
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0</v>
+      </c>
+      <c r="K15" s="5">
+        <v>1</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
+      <c r="N15" s="5">
+        <v>0</v>
+      </c>
+      <c r="O15" s="5">
+        <v>0</v>
+      </c>
+      <c r="P15" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="6">
-        <v>0</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0</v>
-      </c>
-      <c r="E16" s="6">
-        <v>0</v>
-      </c>
-      <c r="F16" s="6">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6">
-        <v>0</v>
-      </c>
-      <c r="I16" s="6">
-        <v>0</v>
-      </c>
-      <c r="J16" s="6">
-        <v>0</v>
-      </c>
-      <c r="K16" s="6">
-        <v>0</v>
-      </c>
-      <c r="L16" s="6">
-        <v>0</v>
-      </c>
-      <c r="M16" s="6">
-        <v>0</v>
-      </c>
-      <c r="N16" s="6">
-        <v>0</v>
-      </c>
-      <c r="O16" s="6">
-        <v>0</v>
-      </c>
-      <c r="P16" s="6">
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0</v>
+      </c>
+      <c r="P16" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3597,896 +3588,896 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="6"/>
+      <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0</v>
-      </c>
-      <c r="K2" s="6">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6">
-        <v>0</v>
-      </c>
-      <c r="M2" s="6">
-        <v>0</v>
-      </c>
-      <c r="N2" s="6">
-        <v>0</v>
-      </c>
-      <c r="O2" s="6">
-        <v>0</v>
-      </c>
-      <c r="P2" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="6"/>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0</v>
-      </c>
-      <c r="M3" s="6">
-        <v>0</v>
-      </c>
-      <c r="N3" s="6">
-        <v>0</v>
-      </c>
-      <c r="O3" s="6">
-        <v>0</v>
-      </c>
-      <c r="P3" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="6"/>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>1</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>1</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
-      <c r="O4" s="6">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6"/>
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6"/>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0</v>
-      </c>
-      <c r="O6" s="6">
-        <v>0</v>
-      </c>
-      <c r="P6" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="6"/>
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0</v>
-      </c>
-      <c r="K7" s="6">
-        <v>0</v>
-      </c>
-      <c r="L7" s="6">
-        <v>0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0</v>
-      </c>
-      <c r="N7" s="6">
-        <v>0</v>
-      </c>
-      <c r="O7" s="6">
-        <v>0</v>
-      </c>
-      <c r="P7" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="6"/>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1</v>
-      </c>
-      <c r="L8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="6">
-        <v>1</v>
-      </c>
-      <c r="N8" s="6">
-        <v>0</v>
-      </c>
-      <c r="O8" s="6">
-        <v>1</v>
-      </c>
-      <c r="P8" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="6"/>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1</v>
+      </c>
+      <c r="P8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <v>1</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
-        <v>0</v>
-      </c>
-      <c r="L9" s="6">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0</v>
-      </c>
-      <c r="O9" s="6">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="6"/>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="5">
+        <v>0</v>
+      </c>
+      <c r="P9" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6">
-        <v>0</v>
-      </c>
-      <c r="N10" s="6">
-        <v>0</v>
-      </c>
-      <c r="O10" s="6">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="6"/>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6">
-        <v>1</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
-        <v>0</v>
-      </c>
-      <c r="N11" s="6">
-        <v>0</v>
-      </c>
-      <c r="O11" s="6">
-        <v>0</v>
-      </c>
-      <c r="P11" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="6"/>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="5">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="6">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6">
-        <v>1</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0</v>
-      </c>
-      <c r="K12" s="6">
-        <v>1</v>
-      </c>
-      <c r="L12" s="6">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
-        <v>1</v>
-      </c>
-      <c r="N12" s="6">
-        <v>0</v>
-      </c>
-      <c r="O12" s="6">
-        <v>0</v>
-      </c>
-      <c r="P12" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="6"/>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>1</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="O12" s="5">
+        <v>0</v>
+      </c>
+      <c r="P12" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="5"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="6">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
-        <v>0</v>
-      </c>
-      <c r="I13" s="6">
-        <v>0</v>
-      </c>
-      <c r="J13" s="6">
-        <v>0</v>
-      </c>
-      <c r="K13" s="6">
-        <v>1</v>
-      </c>
-      <c r="L13" s="6">
-        <v>0</v>
-      </c>
-      <c r="M13" s="6">
-        <v>0</v>
-      </c>
-      <c r="N13" s="6">
-        <v>0</v>
-      </c>
-      <c r="O13" s="6">
-        <v>1</v>
-      </c>
-      <c r="P13" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="6"/>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5">
+        <v>1</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+      <c r="O13" s="5">
+        <v>1</v>
+      </c>
+      <c r="P13" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6">
-        <v>1</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0</v>
-      </c>
-      <c r="I14" s="6">
-        <v>0</v>
-      </c>
-      <c r="J14" s="6">
-        <v>0</v>
-      </c>
-      <c r="K14" s="6">
-        <v>1</v>
-      </c>
-      <c r="L14" s="6">
-        <v>0</v>
-      </c>
-      <c r="M14" s="6">
-        <v>0</v>
-      </c>
-      <c r="N14" s="6">
-        <v>0</v>
-      </c>
-      <c r="O14" s="6">
-        <v>0</v>
-      </c>
-      <c r="P14" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="6"/>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5">
+        <v>1</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+      <c r="O14" s="5">
+        <v>0</v>
+      </c>
+      <c r="P14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="5"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="6">
-        <v>1</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0</v>
-      </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0</v>
-      </c>
-      <c r="I15" s="6">
-        <v>0</v>
-      </c>
-      <c r="J15" s="6">
-        <v>0</v>
-      </c>
-      <c r="K15" s="6">
-        <v>1</v>
-      </c>
-      <c r="L15" s="6">
-        <v>0</v>
-      </c>
-      <c r="M15" s="6">
-        <v>0</v>
-      </c>
-      <c r="N15" s="6">
-        <v>0</v>
-      </c>
-      <c r="O15" s="6">
-        <v>0</v>
-      </c>
-      <c r="P15" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="6"/>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0</v>
+      </c>
+      <c r="K15" s="5">
+        <v>1</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
+      <c r="N15" s="5">
+        <v>0</v>
+      </c>
+      <c r="O15" s="5">
+        <v>0</v>
+      </c>
+      <c r="P15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="6">
-        <v>0</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0</v>
-      </c>
-      <c r="E16" s="6">
-        <v>0</v>
-      </c>
-      <c r="F16" s="6">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6">
-        <v>0</v>
-      </c>
-      <c r="I16" s="6">
-        <v>0</v>
-      </c>
-      <c r="J16" s="6">
-        <v>0</v>
-      </c>
-      <c r="K16" s="6">
-        <v>0</v>
-      </c>
-      <c r="L16" s="6">
-        <v>0</v>
-      </c>
-      <c r="M16" s="6">
-        <v>0</v>
-      </c>
-      <c r="N16" s="6">
-        <v>0</v>
-      </c>
-      <c r="O16" s="6">
-        <v>0</v>
-      </c>
-      <c r="P16" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="6"/>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0</v>
+      </c>
+      <c r="P16" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="5"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4501,10 +4492,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4515,171 +4506,180 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="3">
-        <v>2E-3</v>
+        <v>38</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="9">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3">
-        <v>100000000</v>
+        <v>14</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="3">
-        <v>9.9999999999999995E-7</v>
+        <v>15</v>
+      </c>
+      <c r="B4" s="9">
+        <v>100000000</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3">
-        <v>100000000</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="9">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="3">
-        <v>9.9999999999999995E-7</v>
+        <v>17</v>
+      </c>
+      <c r="B6" s="9">
+        <v>100000000</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="9">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="5">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="5">
+        <v>22</v>
+      </c>
+      <c r="B10" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="5">
+        <v>24</v>
+      </c>
+      <c r="B12" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="5">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1">
-        <v>30</v>
-      </c>
-      <c r="D13" s="1">
-        <v>60</v>
+        <v>25</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
+      </c>
+      <c r="B14" s="4">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
         <v>5</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <v>10</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="1">
         <v>15</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F16" s="1">
         <v>20</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G16" s="1">
         <v>25</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H16" s="1">
         <v>30</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I16" s="1">
         <v>35</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J16" s="1">
         <v>40</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K16" s="1">
         <v>45</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L16" s="1">
         <v>50</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M16" s="1">
         <v>55</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N16" s="1">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4692,7 +4692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -4710,7 +4710,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1">
@@ -4718,7 +4718,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1">
@@ -4726,7 +4726,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1">
@@ -4734,7 +4734,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="1">
@@ -4742,7 +4742,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1">
@@ -4750,7 +4750,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1">
@@ -4758,7 +4758,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1">
@@ -4766,7 +4766,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1">
@@ -4774,7 +4774,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="1">
@@ -4782,7 +4782,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1">
@@ -4790,7 +4790,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1">
@@ -4798,7 +4798,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="1">
@@ -4806,7 +4806,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="1">
@@ -4814,7 +4814,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="1">
@@ -4822,7 +4822,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="1">

</xml_diff>